<commit_message>
placement 3 and 9
</commit_message>
<xml_diff>
--- a/day2/placement/data/data_maker/result.xlsx
+++ b/day2/placement/data/data_maker/result.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6E77AC83-CEB7-416D-8951-4BDC8204D946}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laekov/oi/problemmaker/CTSC2018/day2/placement/data/data_maker/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,18 +48,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -82,7 +89,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,19 +366,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1">
         <v>1</v>
       </c>
@@ -403,13 +410,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>317</v>
       </c>
+      <c r="C2">
+        <v>114</v>
+      </c>
+      <c r="D2">
+        <v>106</v>
+      </c>
       <c r="E2">
         <v>50544</v>
       </c>
@@ -419,17 +432,26 @@
       <c r="G2">
         <v>3575327</v>
       </c>
+      <c r="J2">
+        <v>21649</v>
+      </c>
       <c r="K2">
         <v>5110163</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>329</v>
       </c>
+      <c r="C3">
+        <v>346</v>
+      </c>
+      <c r="D3">
+        <v>456</v>
+      </c>
       <c r="E3">
         <v>70491</v>
       </c>
@@ -439,17 +461,26 @@
       <c r="G3">
         <v>6339468</v>
       </c>
+      <c r="J3">
+        <v>113030</v>
+      </c>
       <c r="K3">
         <v>6473766</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>326</v>
       </c>
+      <c r="C4">
+        <v>358</v>
+      </c>
+      <c r="D4">
+        <v>462</v>
+      </c>
       <c r="E4">
         <v>70963</v>
       </c>
@@ -459,17 +490,26 @@
       <c r="G4">
         <v>6370345</v>
       </c>
+      <c r="J4">
+        <v>288016</v>
+      </c>
       <c r="K4">
         <v>6382056</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>320</v>
       </c>
+      <c r="C5">
+        <v>232</v>
+      </c>
+      <c r="D5">
+        <v>307</v>
+      </c>
       <c r="E5">
         <v>50617</v>
       </c>
@@ -478,6 +518,9 @@
       </c>
       <c r="G5">
         <v>6007740</v>
+      </c>
+      <c r="J5">
+        <v>144417</v>
       </c>
       <c r="K5">
         <v>5110629</v>

</xml_diff>

<commit_message>
replacement fix simulator bug and update answers
</commit_message>
<xml_diff>
--- a/day2/placement/data/data_maker/result.xlsx
+++ b/day2/placement/data/data_maker/result.xlsx
@@ -370,7 +370,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -418,7 +418,7 @@
         <v>317</v>
       </c>
       <c r="C2">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D2">
         <v>106</v>
@@ -439,7 +439,7 @@
         <v>4977</v>
       </c>
       <c r="J2">
-        <v>21429</v>
+        <v>22328</v>
       </c>
       <c r="K2">
         <v>5110163</v>
@@ -474,7 +474,7 @@
         <v>337807</v>
       </c>
       <c r="J3">
-        <v>53398</v>
+        <v>113030</v>
       </c>
       <c r="K3">
         <v>6473766</v>
@@ -503,13 +503,13 @@
         <v>6370345</v>
       </c>
       <c r="H4">
-        <v>732696</v>
+        <v>7824</v>
       </c>
       <c r="I4">
         <v>14192</v>
       </c>
       <c r="J4">
-        <v>8225</v>
+        <v>30017</v>
       </c>
       <c r="K4">
         <v>6382056</v>
@@ -538,13 +538,13 @@
         <v>6007740</v>
       </c>
       <c r="H5">
-        <v>502615</v>
+        <v>5031</v>
       </c>
       <c r="I5">
-        <v>8330</v>
+        <v>8331</v>
       </c>
       <c r="J5">
-        <v>5031</v>
+        <v>53398</v>
       </c>
       <c r="K5">
         <v>5110629</v>

</xml_diff>

<commit_message>
update replacement 9 best
</commit_message>
<xml_diff>
--- a/day2/placement/data/data_maker/result.xlsx
+++ b/day2/placement/data/data_maker/result.xlsx
@@ -370,7 +370,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -418,7 +418,7 @@
         <v>317</v>
       </c>
       <c r="C2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2">
         <v>106</v>
@@ -439,7 +439,7 @@
         <v>4977</v>
       </c>
       <c r="J2">
-        <v>22328</v>
+        <v>21819</v>
       </c>
       <c r="K2">
         <v>5110163</v>

</xml_diff>